<commit_message>
New files so merged end times are different
</commit_message>
<xml_diff>
--- a/test2/stats.xlsx
+++ b/test2/stats.xlsx
@@ -466,28 +466,28 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="F3" t="n">
-        <v>135</v>
+        <v>116</v>
       </c>
       <c r="G3" t="n">
-        <v>189</v>
+        <v>242</v>
       </c>
       <c r="H3" t="n">
-        <v>115</v>
+        <v>214</v>
       </c>
       <c r="I3" t="n">
-        <v>192</v>
+        <v>261</v>
       </c>
       <c r="J3" t="n">
-        <v>425</v>
+        <v>188</v>
       </c>
       <c r="K3" t="n">
-        <v>120</v>
+        <v>172</v>
       </c>
       <c r="L3" t="n">
-        <v>19</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4">
@@ -497,28 +497,28 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>130</v>
+        <v>240</v>
       </c>
       <c r="F4" t="n">
-        <v>117</v>
+        <v>2</v>
       </c>
       <c r="G4" t="n">
-        <v>12</v>
+        <v>62</v>
       </c>
       <c r="H4" t="n">
-        <v>169</v>
+        <v>115</v>
       </c>
       <c r="I4" t="n">
-        <v>55</v>
+        <v>23</v>
       </c>
       <c r="J4" t="n">
-        <v>78</v>
+        <v>46</v>
       </c>
       <c r="K4" t="n">
-        <v>151</v>
+        <v>99</v>
       </c>
       <c r="L4" t="n">
-        <v>279</v>
+        <v>239</v>
       </c>
     </row>
     <row r="5">
@@ -533,28 +533,28 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>27404</v>
+        <v>16602</v>
       </c>
       <c r="F5" t="n">
-        <v>158326</v>
+        <v>79904</v>
       </c>
       <c r="G5" t="n">
-        <v>350450</v>
+        <v>404651</v>
       </c>
       <c r="H5" t="n">
-        <v>214733</v>
+        <v>580478</v>
       </c>
       <c r="I5" t="n">
-        <v>259321</v>
+        <v>389079</v>
       </c>
       <c r="J5" t="n">
-        <v>4746405</v>
+        <v>754174</v>
       </c>
       <c r="K5" t="n">
-        <v>3796298</v>
+        <v>3365151</v>
       </c>
       <c r="L5" t="n">
-        <v>25916</v>
+        <v>15334</v>
       </c>
     </row>
     <row r="6">
@@ -564,28 +564,28 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>100644</v>
+        <v>1748671</v>
       </c>
       <c r="F6" t="n">
-        <v>88606</v>
+        <v>954</v>
       </c>
       <c r="G6" t="n">
-        <v>5938</v>
+        <v>128148</v>
       </c>
       <c r="H6" t="n">
-        <v>4726407</v>
+        <v>2735201</v>
       </c>
       <c r="I6" t="n">
-        <v>98776</v>
+        <v>22029</v>
       </c>
       <c r="J6" t="n">
-        <v>4074685</v>
+        <v>4118116</v>
       </c>
       <c r="K6" t="n">
-        <v>219310</v>
+        <v>104670</v>
       </c>
       <c r="L6" t="n">
-        <v>3480073</v>
+        <v>195624</v>
       </c>
     </row>
     <row r="7">
@@ -600,28 +600,28 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>474</v>
+        <v>467</v>
       </c>
       <c r="F7" t="n">
-        <v>474</v>
+        <v>464</v>
       </c>
       <c r="G7" t="n">
         <v>459</v>
       </c>
       <c r="H7" t="n">
+        <v>463</v>
+      </c>
+      <c r="I7" t="n">
+        <v>461</v>
+      </c>
+      <c r="J7" t="n">
+        <v>461</v>
+      </c>
+      <c r="K7" t="n">
+        <v>466</v>
+      </c>
+      <c r="L7" t="n">
         <v>469</v>
-      </c>
-      <c r="I7" t="n">
-        <v>467</v>
-      </c>
-      <c r="J7" t="n">
-        <v>440</v>
-      </c>
-      <c r="K7" t="n">
-        <v>459</v>
-      </c>
-      <c r="L7" t="n">
-        <v>463</v>
       </c>
     </row>
     <row r="8">
@@ -631,28 +631,28 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>472</v>
+        <v>462</v>
       </c>
       <c r="F8" t="n">
-        <v>474</v>
+        <v>477</v>
       </c>
       <c r="G8" t="n">
+        <v>463</v>
+      </c>
+      <c r="H8" t="n">
+        <v>467</v>
+      </c>
+      <c r="I8" t="n">
         <v>469</v>
       </c>
-      <c r="H8" t="n">
-        <v>471</v>
-      </c>
-      <c r="I8" t="n">
-        <v>477</v>
-      </c>
       <c r="J8" t="n">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="K8" t="n">
+        <v>463</v>
+      </c>
+      <c r="L8" t="n">
         <v>462</v>
-      </c>
-      <c r="L8" t="n">
-        <v>461</v>
       </c>
     </row>
     <row r="9">
@@ -667,28 +667,28 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>2035</v>
+        <v>818</v>
       </c>
       <c r="F9" t="n">
-        <v>6538</v>
+        <v>6734</v>
       </c>
       <c r="G9" t="n">
         <v>206746</v>
       </c>
       <c r="H9" t="n">
-        <v>16488</v>
+        <v>26689</v>
       </c>
       <c r="I9" t="n">
-        <v>15161</v>
+        <v>16527</v>
       </c>
       <c r="J9" t="n">
-        <v>3224909</v>
+        <v>408297</v>
       </c>
       <c r="K9" t="n">
         <v>2844365</v>
       </c>
       <c r="L9" t="n">
-        <v>16696</v>
+        <v>1859</v>
       </c>
     </row>
     <row r="10">
@@ -698,28 +698,28 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>14995</v>
+        <v>907406</v>
       </c>
       <c r="F10" t="n">
-        <v>4842</v>
+        <v>477</v>
       </c>
       <c r="G10" t="n">
-        <v>639</v>
+        <v>96784</v>
       </c>
       <c r="H10" t="n">
         <v>1126123</v>
       </c>
       <c r="I10" t="n">
-        <v>11670</v>
+        <v>9063</v>
       </c>
       <c r="J10" t="n">
-        <v>2252083</v>
+        <v>3808470</v>
       </c>
       <c r="K10" t="n">
-        <v>16777</v>
+        <v>14510</v>
       </c>
       <c r="L10" t="n">
-        <v>801120</v>
+        <v>36436</v>
       </c>
     </row>
     <row r="11">
@@ -734,28 +734,28 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>595.7391304347826</v>
+        <v>503.0909090909091</v>
       </c>
       <c r="F11" t="n">
-        <v>1172.785185185185</v>
+        <v>688.8275862068965</v>
       </c>
       <c r="G11" t="n">
-        <v>1854.232804232804</v>
+        <v>1672.111570247934</v>
       </c>
       <c r="H11" t="n">
-        <v>1867.24347826087</v>
+        <v>2712.514018691589</v>
       </c>
       <c r="I11" t="n">
-        <v>1350.630208333333</v>
+        <v>1490.724137931034</v>
       </c>
       <c r="J11" t="n">
-        <v>11168.01176470588</v>
+        <v>4011.563829787234</v>
       </c>
       <c r="K11" t="n">
-        <v>31635.81666666667</v>
+        <v>19564.83139534884</v>
       </c>
       <c r="L11" t="n">
-        <v>1364</v>
+        <v>528.7586206896551</v>
       </c>
     </row>
     <row r="12">
@@ -765,28 +765,28 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>774.1846153846154</v>
+        <v>7286.129166666667</v>
       </c>
       <c r="F12" t="n">
-        <v>757.3162393162393</v>
+        <v>477</v>
       </c>
       <c r="G12" t="n">
-        <v>494.8333333333333</v>
+        <v>2066.903225806452</v>
       </c>
       <c r="H12" t="n">
-        <v>27966.90532544379</v>
+        <v>23784.35652173913</v>
       </c>
       <c r="I12" t="n">
-        <v>1795.927272727273</v>
+        <v>957.7826086956521</v>
       </c>
       <c r="J12" t="n">
-        <v>52239.55128205128</v>
+        <v>89524.26086956522</v>
       </c>
       <c r="K12" t="n">
-        <v>1452.384105960265</v>
+        <v>1057.272727272727</v>
       </c>
       <c r="L12" t="n">
-        <v>12473.37992831541</v>
+        <v>818.510460251046</v>
       </c>
     </row>
     <row r="13">
@@ -801,19 +801,19 @@
         </is>
       </c>
       <c r="E13" t="n">
-        <v>479</v>
+        <v>470</v>
       </c>
       <c r="F13" t="n">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="G13" t="n">
-        <v>469</v>
+        <v>469.25</v>
       </c>
       <c r="H13" t="n">
-        <v>479</v>
+        <v>471</v>
       </c>
       <c r="I13" t="n">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="J13" t="n">
         <v>470</v>
@@ -832,19 +832,19 @@
         </is>
       </c>
       <c r="E14" t="n">
-        <v>479</v>
+        <v>470</v>
       </c>
       <c r="F14" t="n">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="G14" t="n">
         <v>470</v>
       </c>
       <c r="H14" t="n">
-        <v>480</v>
+        <v>473</v>
       </c>
       <c r="I14" t="n">
-        <v>479</v>
+        <v>470</v>
       </c>
       <c r="J14" t="n">
         <v>470</v>
@@ -868,25 +868,25 @@
         </is>
       </c>
       <c r="E15" t="n">
-        <v>480.5</v>
+        <v>479</v>
       </c>
       <c r="F15" t="n">
-        <v>483</v>
+        <v>477</v>
       </c>
       <c r="G15" t="n">
-        <v>470</v>
+        <v>476</v>
       </c>
       <c r="H15" t="n">
-        <v>487</v>
+        <v>481</v>
       </c>
       <c r="I15" t="n">
-        <v>488</v>
+        <v>480</v>
       </c>
       <c r="J15" t="n">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="K15" t="n">
-        <v>472</v>
+        <v>479</v>
       </c>
       <c r="L15" t="n">
         <v>471</v>
@@ -899,28 +899,28 @@
         </is>
       </c>
       <c r="E16" t="n">
-        <v>481</v>
+        <v>470</v>
       </c>
       <c r="F16" t="n">
-        <v>486</v>
+        <v>477</v>
       </c>
       <c r="G16" t="n">
-        <v>470</v>
+        <v>476</v>
       </c>
       <c r="H16" t="n">
-        <v>503</v>
+        <v>587</v>
       </c>
       <c r="I16" t="n">
-        <v>491</v>
+        <v>477</v>
       </c>
       <c r="J16" t="n">
         <v>471</v>
       </c>
       <c r="K16" t="n">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="L16" t="n">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="17">
@@ -935,28 +935,28 @@
         </is>
       </c>
       <c r="E17" t="n">
-        <v>492.5</v>
+        <v>488</v>
       </c>
       <c r="F17" t="n">
-        <v>918</v>
+        <v>478</v>
       </c>
       <c r="G17" t="n">
-        <v>485</v>
+        <v>588.75</v>
       </c>
       <c r="H17" t="n">
-        <v>1503.5</v>
+        <v>2203.5</v>
       </c>
       <c r="I17" t="n">
-        <v>1031.75</v>
+        <v>1194</v>
       </c>
       <c r="J17" t="n">
-        <v>1194</v>
+        <v>1120.5</v>
       </c>
       <c r="K17" t="n">
-        <v>1135.75</v>
+        <v>648.5</v>
       </c>
       <c r="L17" t="n">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="18">
@@ -966,28 +966,28 @@
         </is>
       </c>
       <c r="E18" t="n">
-        <v>490</v>
+        <v>479</v>
       </c>
       <c r="F18" t="n">
-        <v>641</v>
+        <v>477</v>
       </c>
       <c r="G18" t="n">
-        <v>474.75</v>
+        <v>480</v>
       </c>
       <c r="H18" t="n">
-        <v>2894</v>
+        <v>2986</v>
       </c>
       <c r="I18" t="n">
-        <v>1394</v>
+        <v>479</v>
       </c>
       <c r="J18" t="n">
         <v>530.75</v>
       </c>
       <c r="K18" t="n">
-        <v>1195</v>
+        <v>746.5</v>
       </c>
       <c r="L18" t="n">
-        <v>587</v>
+        <v>480</v>
       </c>
     </row>
     <row r="19">
@@ -1002,28 +1002,28 @@
         </is>
       </c>
       <c r="E19" t="n">
-        <v>13.5</v>
+        <v>18</v>
       </c>
       <c r="F19" t="n">
-        <v>439</v>
+        <v>2</v>
       </c>
       <c r="G19" t="n">
-        <v>16</v>
+        <v>119.5</v>
       </c>
       <c r="H19" t="n">
-        <v>1024.5</v>
+        <v>1732.5</v>
       </c>
       <c r="I19" t="n">
-        <v>552.75</v>
+        <v>718</v>
       </c>
       <c r="J19" t="n">
-        <v>724</v>
+        <v>650.5</v>
       </c>
       <c r="K19" t="n">
-        <v>665.75</v>
+        <v>178.5</v>
       </c>
       <c r="L19" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20">
@@ -1033,28 +1033,26 @@
         </is>
       </c>
       <c r="E20" t="n">
-        <v>11</v>
-      </c>
-      <c r="F20" t="n">
-        <v>162</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="F20" t="inlineStr"/>
       <c r="G20" t="n">
-        <v>4.75</v>
+        <v>10</v>
       </c>
       <c r="H20" t="n">
-        <v>2414</v>
+        <v>2513</v>
       </c>
       <c r="I20" t="n">
-        <v>915</v>
+        <v>9</v>
       </c>
       <c r="J20" t="n">
         <v>60.75</v>
       </c>
       <c r="K20" t="n">
-        <v>725</v>
+        <v>276.5</v>
       </c>
       <c r="L20" t="n">
-        <v>117</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23">
@@ -1102,28 +1100,28 @@
         </is>
       </c>
       <c r="E25" t="n">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="F25" t="n">
-        <v>135</v>
+        <v>115</v>
       </c>
       <c r="G25" t="n">
-        <v>189</v>
+        <v>241</v>
       </c>
       <c r="H25" t="n">
-        <v>115</v>
+        <v>213</v>
       </c>
       <c r="I25" t="n">
-        <v>192</v>
+        <v>260</v>
       </c>
       <c r="J25" t="n">
-        <v>425</v>
+        <v>187</v>
       </c>
       <c r="K25" t="n">
-        <v>120</v>
+        <v>171</v>
       </c>
       <c r="L25" t="n">
-        <v>19</v>
+        <v>28</v>
       </c>
     </row>
     <row r="26">
@@ -1133,28 +1131,28 @@
         </is>
       </c>
       <c r="E26" t="n">
-        <v>130</v>
+        <v>239</v>
       </c>
       <c r="F26" t="n">
-        <v>117</v>
+        <v>1</v>
       </c>
       <c r="G26" t="n">
-        <v>12</v>
+        <v>61</v>
       </c>
       <c r="H26" t="n">
-        <v>169</v>
+        <v>114</v>
       </c>
       <c r="I26" t="n">
-        <v>55</v>
+        <v>22</v>
       </c>
       <c r="J26" t="n">
-        <v>78</v>
+        <v>45</v>
       </c>
       <c r="K26" t="n">
-        <v>151</v>
+        <v>98</v>
       </c>
       <c r="L26" t="n">
-        <v>279</v>
+        <v>238</v>
       </c>
     </row>
     <row r="27">
@@ -1169,28 +1167,28 @@
         </is>
       </c>
       <c r="E27" t="n">
-        <v>611211</v>
+        <v>134019</v>
       </c>
       <c r="F27" t="n">
-        <v>741117</v>
+        <v>80276</v>
       </c>
       <c r="G27" t="n">
-        <v>10960196</v>
+        <v>225491</v>
       </c>
       <c r="H27" t="n">
-        <v>6874731</v>
+        <v>229176</v>
       </c>
       <c r="I27" t="n">
-        <v>670973</v>
+        <v>230792</v>
       </c>
       <c r="J27" t="n">
-        <v>27854777</v>
+        <v>200653</v>
       </c>
       <c r="K27" t="n">
-        <v>2452713</v>
+        <v>210588</v>
       </c>
       <c r="L27" t="n">
-        <v>12915569</v>
+        <v>197355</v>
       </c>
     </row>
     <row r="28">
@@ -1200,28 +1198,28 @@
         </is>
       </c>
       <c r="E28" t="n">
-        <v>563185</v>
+        <v>144248</v>
       </c>
       <c r="F28" t="n">
-        <v>784411</v>
+        <v>233</v>
       </c>
       <c r="G28" t="n">
-        <v>3654579</v>
+        <v>198562</v>
       </c>
       <c r="H28" t="n">
-        <v>3429335</v>
+        <v>223077</v>
       </c>
       <c r="I28" t="n">
-        <v>771749</v>
+        <v>219744</v>
       </c>
       <c r="J28" t="n">
-        <v>23531159</v>
+        <v>192445</v>
       </c>
       <c r="K28" t="n">
-        <v>6070003</v>
+        <v>213955</v>
       </c>
       <c r="L28" t="n">
-        <v>9487252</v>
+        <v>212586</v>
       </c>
     </row>
     <row r="29">
@@ -1235,30 +1233,16 @@
           <t>Left</t>
         </is>
       </c>
-      <c r="E29" t="n">
-        <v>585</v>
-      </c>
-      <c r="F29" t="n">
-        <v>529</v>
-      </c>
+      <c r="E29" t="inlineStr"/>
+      <c r="F29" t="inlineStr"/>
       <c r="G29" t="n">
-        <v>516</v>
-      </c>
-      <c r="H29" t="n">
-        <v>522</v>
-      </c>
-      <c r="I29" t="n">
-        <v>523</v>
-      </c>
-      <c r="J29" t="n">
-        <v>516</v>
-      </c>
-      <c r="K29" t="n">
-        <v>524</v>
-      </c>
-      <c r="L29" t="n">
-        <v>590</v>
-      </c>
+        <v>-57</v>
+      </c>
+      <c r="H29" t="inlineStr"/>
+      <c r="I29" t="inlineStr"/>
+      <c r="J29" t="inlineStr"/>
+      <c r="K29" t="inlineStr"/>
+      <c r="L29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="C30" t="inlineStr">
@@ -1266,30 +1250,16 @@
           <t>Right</t>
         </is>
       </c>
-      <c r="E30" t="n">
-        <v>531</v>
-      </c>
+      <c r="E30" t="inlineStr"/>
       <c r="F30" t="n">
-        <v>532</v>
-      </c>
-      <c r="G30" t="n">
-        <v>538</v>
-      </c>
-      <c r="H30" t="n">
-        <v>527</v>
-      </c>
-      <c r="I30" t="n">
-        <v>649</v>
-      </c>
-      <c r="J30" t="n">
-        <v>520</v>
-      </c>
-      <c r="K30" t="n">
-        <v>518</v>
-      </c>
-      <c r="L30" t="n">
-        <v>509</v>
-      </c>
+        <v>233</v>
+      </c>
+      <c r="G30" t="inlineStr"/>
+      <c r="H30" t="inlineStr"/>
+      <c r="I30" t="inlineStr"/>
+      <c r="J30" t="inlineStr"/>
+      <c r="K30" t="inlineStr"/>
+      <c r="L30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="B31" t="inlineStr">
@@ -1303,28 +1273,28 @@
         </is>
       </c>
       <c r="E31" t="n">
-        <v>205335</v>
+        <v>35637</v>
       </c>
       <c r="F31" t="n">
-        <v>107818</v>
+        <v>20160</v>
       </c>
       <c r="G31" t="n">
-        <v>7525111</v>
+        <v>16106</v>
       </c>
       <c r="H31" t="n">
-        <v>3088609</v>
+        <v>30070</v>
       </c>
       <c r="I31" t="n">
-        <v>88755</v>
+        <v>31410</v>
       </c>
       <c r="J31" t="n">
-        <v>7780296</v>
+        <v>31910</v>
       </c>
       <c r="K31" t="n">
-        <v>1113541</v>
+        <v>41718</v>
       </c>
       <c r="L31" t="n">
-        <v>12074914</v>
+        <v>109783</v>
       </c>
     </row>
     <row r="32">
@@ -1334,28 +1304,28 @@
         </is>
       </c>
       <c r="E32" t="n">
-        <v>88227</v>
+        <v>21955</v>
       </c>
       <c r="F32" t="n">
-        <v>95141</v>
+        <v>233</v>
       </c>
       <c r="G32" t="n">
-        <v>2513345</v>
+        <v>42468</v>
       </c>
       <c r="H32" t="n">
-        <v>1224777</v>
+        <v>38333</v>
       </c>
       <c r="I32" t="n">
-        <v>259848</v>
+        <v>72522</v>
       </c>
       <c r="J32" t="n">
-        <v>7978815</v>
+        <v>38870</v>
       </c>
       <c r="K32" t="n">
-        <v>4835848</v>
+        <v>51579</v>
       </c>
       <c r="L32" t="n">
-        <v>961188</v>
+        <v>46455</v>
       </c>
     </row>
     <row r="33">
@@ -1370,28 +1340,28 @@
         </is>
       </c>
       <c r="E33" t="n">
-        <v>13287.19565217391</v>
+        <v>4188.09375</v>
       </c>
       <c r="F33" t="n">
-        <v>5489.755555555555</v>
+        <v>698.0521739130435</v>
       </c>
       <c r="G33" t="n">
-        <v>57990.45502645503</v>
+        <v>935.6473029045643</v>
       </c>
       <c r="H33" t="n">
-        <v>59780.26956521739</v>
+        <v>1075.943661971831</v>
       </c>
       <c r="I33" t="n">
-        <v>3494.651041666667</v>
+        <v>887.6615384615385</v>
       </c>
       <c r="J33" t="n">
-        <v>65540.65176470588</v>
+        <v>1073.010695187166</v>
       </c>
       <c r="K33" t="n">
-        <v>20439.275</v>
+        <v>1231.508771929825</v>
       </c>
       <c r="L33" t="n">
-        <v>679766.7894736842</v>
+        <v>7048.392857142857</v>
       </c>
     </row>
     <row r="34">
@@ -1401,28 +1371,28 @@
         </is>
       </c>
       <c r="E34" t="n">
-        <v>4332.192307692308</v>
+        <v>603.5481171548117</v>
       </c>
       <c r="F34" t="n">
-        <v>6704.367521367521</v>
+        <v>233</v>
       </c>
       <c r="G34" t="n">
-        <v>304548.25</v>
+        <v>3255.114754098361</v>
       </c>
       <c r="H34" t="n">
-        <v>20291.92307692308</v>
+        <v>1956.815789473684</v>
       </c>
       <c r="I34" t="n">
-        <v>14031.8</v>
+        <v>9988.363636363636</v>
       </c>
       <c r="J34" t="n">
-        <v>301681.5256410256</v>
+        <v>4276.555555555556</v>
       </c>
       <c r="K34" t="n">
-        <v>40198.69536423841</v>
+        <v>2183.214285714286</v>
       </c>
       <c r="L34" t="n">
-        <v>34004.48745519713</v>
+        <v>893.2184873949579</v>
       </c>
     </row>
     <row r="35">
@@ -1437,28 +1407,28 @@
         </is>
       </c>
       <c r="E35" t="n">
-        <v>1526.5</v>
+        <v>1.75</v>
       </c>
       <c r="F35" t="n">
-        <v>1311</v>
+        <v>1</v>
       </c>
       <c r="G35" t="n">
-        <v>893</v>
+        <v>1</v>
       </c>
       <c r="H35" t="n">
-        <v>960</v>
+        <v>1</v>
       </c>
       <c r="I35" t="n">
-        <v>746.25</v>
+        <v>1</v>
       </c>
       <c r="J35" t="n">
-        <v>918</v>
+        <v>4.5</v>
       </c>
       <c r="K35" t="n">
-        <v>1231</v>
+        <v>2</v>
       </c>
       <c r="L35" t="n">
-        <v>1480</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36">
@@ -1468,28 +1438,28 @@
         </is>
       </c>
       <c r="E36" t="n">
-        <v>1129</v>
+        <v>3</v>
       </c>
       <c r="F36" t="n">
-        <v>1352</v>
+        <v>233</v>
       </c>
       <c r="G36" t="n">
-        <v>1439.5</v>
+        <v>1</v>
       </c>
       <c r="H36" t="n">
-        <v>1029</v>
+        <v>1.25</v>
       </c>
       <c r="I36" t="n">
-        <v>1892</v>
+        <v>4</v>
       </c>
       <c r="J36" t="n">
-        <v>1822.75</v>
+        <v>13</v>
       </c>
       <c r="K36" t="n">
-        <v>648.5</v>
+        <v>1</v>
       </c>
       <c r="L36" t="n">
-        <v>1187</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37">
@@ -1504,28 +1474,28 @@
         </is>
       </c>
       <c r="E37" t="n">
-        <v>2636</v>
+        <v>6</v>
       </c>
       <c r="F37" t="n">
-        <v>1963</v>
+        <v>2</v>
       </c>
       <c r="G37" t="n">
-        <v>1877</v>
+        <v>3</v>
       </c>
       <c r="H37" t="n">
-        <v>1643</v>
+        <v>5</v>
       </c>
       <c r="I37" t="n">
-        <v>1466.5</v>
+        <v>2</v>
       </c>
       <c r="J37" t="n">
-        <v>1580</v>
+        <v>57</v>
       </c>
       <c r="K37" t="n">
-        <v>2477.5</v>
+        <v>4</v>
       </c>
       <c r="L37" t="n">
-        <v>2070</v>
+        <v>6</v>
       </c>
     </row>
     <row r="38">
@@ -1535,28 +1505,28 @@
         </is>
       </c>
       <c r="E38" t="n">
-        <v>2159</v>
+        <v>46</v>
       </c>
       <c r="F38" t="n">
-        <v>1877</v>
+        <v>233</v>
       </c>
       <c r="G38" t="n">
-        <v>10748</v>
+        <v>36</v>
       </c>
       <c r="H38" t="n">
-        <v>2018</v>
+        <v>6</v>
       </c>
       <c r="I38" t="n">
-        <v>3478</v>
+        <v>386</v>
       </c>
       <c r="J38" t="n">
-        <v>6018</v>
+        <v>265</v>
       </c>
       <c r="K38" t="n">
-        <v>1378</v>
+        <v>4</v>
       </c>
       <c r="L38" t="n">
-        <v>2056</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39">
@@ -1571,28 +1541,28 @@
         </is>
       </c>
       <c r="E39" t="n">
-        <v>9227.5</v>
+        <v>3672.25</v>
       </c>
       <c r="F39" t="n">
-        <v>4489.5</v>
+        <v>7</v>
       </c>
       <c r="G39" t="n">
-        <v>3609</v>
+        <v>213</v>
       </c>
       <c r="H39" t="n">
-        <v>3183.5</v>
+        <v>438</v>
       </c>
       <c r="I39" t="n">
-        <v>2403.25</v>
+        <v>8</v>
       </c>
       <c r="J39" t="n">
-        <v>3185</v>
+        <v>676.5</v>
       </c>
       <c r="K39" t="n">
-        <v>7325</v>
+        <v>66.5</v>
       </c>
       <c r="L39" t="n">
-        <v>43898</v>
+        <v>1657.5</v>
       </c>
     </row>
     <row r="40">
@@ -1602,28 +1572,28 @@
         </is>
       </c>
       <c r="E40" t="n">
-        <v>4242</v>
+        <v>174.5</v>
       </c>
       <c r="F40" t="n">
-        <v>3410</v>
+        <v>233</v>
       </c>
       <c r="G40" t="n">
-        <v>283579.75</v>
+        <v>1300</v>
       </c>
       <c r="H40" t="n">
-        <v>6197</v>
+        <v>636.5</v>
       </c>
       <c r="I40" t="n">
-        <v>7788</v>
+        <v>11211.75</v>
       </c>
       <c r="J40" t="n">
-        <v>33736.5</v>
+        <v>2840</v>
       </c>
       <c r="K40" t="n">
-        <v>3091.5</v>
+        <v>205.25</v>
       </c>
       <c r="L40" t="n">
-        <v>5139.5</v>
+        <v>28</v>
       </c>
     </row>
     <row r="41">
@@ -1638,28 +1608,28 @@
         </is>
       </c>
       <c r="E41" t="n">
-        <v>7701</v>
+        <v>3670.5</v>
       </c>
       <c r="F41" t="n">
-        <v>3178.5</v>
+        <v>6</v>
       </c>
       <c r="G41" t="n">
-        <v>2716</v>
+        <v>212</v>
       </c>
       <c r="H41" t="n">
-        <v>2223.5</v>
+        <v>437</v>
       </c>
       <c r="I41" t="n">
-        <v>1657</v>
+        <v>7</v>
       </c>
       <c r="J41" t="n">
-        <v>2267</v>
+        <v>672</v>
       </c>
       <c r="K41" t="n">
-        <v>6094</v>
+        <v>64.5</v>
       </c>
       <c r="L41" t="n">
-        <v>42418</v>
+        <v>1656.5</v>
       </c>
     </row>
     <row r="42">
@@ -1669,28 +1639,26 @@
         </is>
       </c>
       <c r="E42" t="n">
-        <v>3113</v>
-      </c>
-      <c r="F42" t="n">
-        <v>2058</v>
-      </c>
+        <v>171.5</v>
+      </c>
+      <c r="F42" t="inlineStr"/>
       <c r="G42" t="n">
-        <v>282140.25</v>
+        <v>1299</v>
       </c>
       <c r="H42" t="n">
-        <v>5168</v>
+        <v>635.25</v>
       </c>
       <c r="I42" t="n">
-        <v>5896</v>
+        <v>11207.75</v>
       </c>
       <c r="J42" t="n">
-        <v>31913.75</v>
+        <v>2827</v>
       </c>
       <c r="K42" t="n">
-        <v>2443</v>
+        <v>204.25</v>
       </c>
       <c r="L42" t="n">
-        <v>3952.5</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Include 90, 95, 99th percentiles and total per device and data set totals
</commit_message>
<xml_diff>
--- a/test2/stats.xlsx
+++ b/test2/stats.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L42"/>
+  <dimension ref="A1:M82"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1055,43 +1055,144 @@
         <v>10</v>
       </c>
     </row>
+    <row r="21">
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>P90</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Left</t>
+        </is>
+      </c>
+      <c r="E21" t="n">
+        <v>491</v>
+      </c>
+      <c r="F21" t="n">
+        <v>593</v>
+      </c>
+      <c r="G21" t="n">
+        <v>1125.7</v>
+      </c>
+      <c r="H21" t="n">
+        <v>8466.800000000007</v>
+      </c>
+      <c r="I21" t="n">
+        <v>4060</v>
+      </c>
+      <c r="J21" t="n">
+        <v>4882.800000000004</v>
+      </c>
+      <c r="K21" t="n">
+        <v>1947.900000000001</v>
+      </c>
+      <c r="L21" t="n">
+        <v>482.4</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Right</t>
+        </is>
+      </c>
+      <c r="E22" t="n">
+        <v>551.7999999999997</v>
+      </c>
+      <c r="F22" t="n">
+        <v>477</v>
+      </c>
+      <c r="G22" t="n">
+        <v>637.5</v>
+      </c>
+      <c r="H22" t="n">
+        <v>8228.000000000013</v>
+      </c>
+      <c r="I22" t="n">
+        <v>1039.200000000001</v>
+      </c>
+      <c r="J22" t="n">
+        <v>1335.5</v>
+      </c>
+      <c r="K22" t="n">
+        <v>1839.8</v>
+      </c>
+      <c r="L22" t="n">
+        <v>880.4000000000016</v>
+      </c>
+    </row>
     <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>Interbouts</t>
-        </is>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>P95</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Left</t>
+        </is>
+      </c>
+      <c r="E23" t="n">
+        <v>714.9999999999998</v>
+      </c>
+      <c r="F23" t="n">
+        <v>1401</v>
+      </c>
+      <c r="G23" t="n">
+        <v>2070.449999999999</v>
+      </c>
+      <c r="H23" t="n">
+        <v>12197.9</v>
+      </c>
+      <c r="I23" t="n">
+        <v>5781</v>
+      </c>
+      <c r="J23" t="n">
+        <v>8730.050000000003</v>
+      </c>
+      <c r="K23" t="n">
+        <v>3588.549999999999</v>
+      </c>
+      <c r="L23" t="n">
+        <v>615.7999999999995</v>
       </c>
     </row>
     <row r="24">
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Right</t>
+        </is>
+      </c>
       <c r="E24" t="n">
-        <v>1</v>
+        <v>798.5999999999998</v>
       </c>
       <c r="F24" t="n">
-        <v>3</v>
+        <v>477</v>
       </c>
       <c r="G24" t="n">
-        <v>5</v>
+        <v>742.4999999999998</v>
       </c>
       <c r="H24" t="n">
-        <v>6</v>
+        <v>62624.49999999961</v>
       </c>
       <c r="I24" t="n">
-        <v>7</v>
+        <v>2176.099999999999</v>
       </c>
       <c r="J24" t="n">
-        <v>8</v>
+        <v>3882</v>
       </c>
       <c r="K24" t="n">
-        <v>9</v>
+        <v>4008.299999999998</v>
       </c>
       <c r="L24" t="n">
-        <v>12</v>
+        <v>1422.9</v>
       </c>
     </row>
     <row r="25">
       <c r="B25" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>P99</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1100,28 +1201,28 @@
         </is>
       </c>
       <c r="E25" t="n">
-        <v>32</v>
+        <v>812.88</v>
       </c>
       <c r="F25" t="n">
-        <v>115</v>
+        <v>6157.999999999992</v>
       </c>
       <c r="G25" t="n">
-        <v>241</v>
+        <v>10846.52000000001</v>
       </c>
       <c r="H25" t="n">
-        <v>213</v>
+        <v>22593.30000000001</v>
       </c>
       <c r="I25" t="n">
-        <v>260</v>
+        <v>10622.59999999997</v>
       </c>
       <c r="J25" t="n">
-        <v>187</v>
+        <v>19176.22999999976</v>
       </c>
       <c r="K25" t="n">
-        <v>171</v>
+        <v>124343.8599999979</v>
       </c>
       <c r="L25" t="n">
-        <v>28</v>
+        <v>1534.759999999999</v>
       </c>
     </row>
     <row r="26">
@@ -1131,140 +1232,67 @@
         </is>
       </c>
       <c r="E26" t="n">
-        <v>239</v>
+        <v>11156.22999999985</v>
       </c>
       <c r="F26" t="n">
+        <v>477</v>
+      </c>
+      <c r="G26" t="n">
+        <v>38462.51000000005</v>
+      </c>
+      <c r="H26" t="n">
+        <v>393705.7999999999</v>
+      </c>
+      <c r="I26" t="n">
+        <v>7572.280000000008</v>
+      </c>
+      <c r="J26" t="n">
+        <v>2220166.19999999</v>
+      </c>
+      <c r="K26" t="n">
+        <v>7158.03999999997</v>
+      </c>
+      <c r="L26" t="n">
+        <v>6066.440000000015</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Interbouts</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="E30" t="n">
         <v>1</v>
       </c>
-      <c r="G26" t="n">
-        <v>61</v>
-      </c>
-      <c r="H26" t="n">
-        <v>114</v>
-      </c>
-      <c r="I26" t="n">
-        <v>22</v>
-      </c>
-      <c r="J26" t="n">
-        <v>45</v>
-      </c>
-      <c r="K26" t="n">
-        <v>98</v>
-      </c>
-      <c r="L26" t="n">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>Sum</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>Left</t>
-        </is>
-      </c>
-      <c r="E27" t="n">
-        <v>134019</v>
-      </c>
-      <c r="F27" t="n">
-        <v>80276</v>
-      </c>
-      <c r="G27" t="n">
-        <v>225491</v>
-      </c>
-      <c r="H27" t="n">
-        <v>229176</v>
-      </c>
-      <c r="I27" t="n">
-        <v>230792</v>
-      </c>
-      <c r="J27" t="n">
-        <v>200653</v>
-      </c>
-      <c r="K27" t="n">
-        <v>210588</v>
-      </c>
-      <c r="L27" t="n">
-        <v>197355</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>Right</t>
-        </is>
-      </c>
-      <c r="E28" t="n">
-        <v>144248</v>
-      </c>
-      <c r="F28" t="n">
-        <v>233</v>
-      </c>
-      <c r="G28" t="n">
-        <v>198562</v>
-      </c>
-      <c r="H28" t="n">
-        <v>223077</v>
-      </c>
-      <c r="I28" t="n">
-        <v>219744</v>
-      </c>
-      <c r="J28" t="n">
-        <v>192445</v>
-      </c>
-      <c r="K28" t="n">
-        <v>213955</v>
-      </c>
-      <c r="L28" t="n">
-        <v>212586</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>Min</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>Left</t>
-        </is>
-      </c>
-      <c r="E29" t="inlineStr"/>
-      <c r="F29" t="inlineStr"/>
-      <c r="G29" t="n">
-        <v>-57</v>
-      </c>
-      <c r="H29" t="inlineStr"/>
-      <c r="I29" t="inlineStr"/>
-      <c r="J29" t="inlineStr"/>
-      <c r="K29" t="inlineStr"/>
-      <c r="L29" t="inlineStr"/>
-    </row>
-    <row r="30">
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>Right</t>
-        </is>
-      </c>
-      <c r="E30" t="inlineStr"/>
       <c r="F30" t="n">
-        <v>233</v>
-      </c>
-      <c r="G30" t="inlineStr"/>
-      <c r="H30" t="inlineStr"/>
-      <c r="I30" t="inlineStr"/>
-      <c r="J30" t="inlineStr"/>
-      <c r="K30" t="inlineStr"/>
-      <c r="L30" t="inlineStr"/>
+        <v>3</v>
+      </c>
+      <c r="G30" t="n">
+        <v>5</v>
+      </c>
+      <c r="H30" t="n">
+        <v>6</v>
+      </c>
+      <c r="I30" t="n">
+        <v>7</v>
+      </c>
+      <c r="J30" t="n">
+        <v>8</v>
+      </c>
+      <c r="K30" t="n">
+        <v>9</v>
+      </c>
+      <c r="L30" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="31">
       <c r="B31" t="inlineStr">
         <is>
-          <t>Max</t>
+          <t>N</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1273,28 +1301,28 @@
         </is>
       </c>
       <c r="E31" t="n">
-        <v>35637</v>
+        <v>32</v>
       </c>
       <c r="F31" t="n">
-        <v>20160</v>
+        <v>115</v>
       </c>
       <c r="G31" t="n">
-        <v>16106</v>
+        <v>241</v>
       </c>
       <c r="H31" t="n">
-        <v>30070</v>
+        <v>213</v>
       </c>
       <c r="I31" t="n">
-        <v>31410</v>
+        <v>260</v>
       </c>
       <c r="J31" t="n">
-        <v>31910</v>
+        <v>187</v>
       </c>
       <c r="K31" t="n">
-        <v>41718</v>
+        <v>171</v>
       </c>
       <c r="L31" t="n">
-        <v>109783</v>
+        <v>28</v>
       </c>
     </row>
     <row r="32">
@@ -1304,34 +1332,34 @@
         </is>
       </c>
       <c r="E32" t="n">
-        <v>21955</v>
+        <v>239</v>
       </c>
       <c r="F32" t="n">
-        <v>233</v>
+        <v>1</v>
       </c>
       <c r="G32" t="n">
-        <v>42468</v>
+        <v>61</v>
       </c>
       <c r="H32" t="n">
-        <v>38333</v>
+        <v>114</v>
       </c>
       <c r="I32" t="n">
-        <v>72522</v>
+        <v>22</v>
       </c>
       <c r="J32" t="n">
-        <v>38870</v>
+        <v>45</v>
       </c>
       <c r="K32" t="n">
-        <v>51579</v>
+        <v>98</v>
       </c>
       <c r="L32" t="n">
-        <v>46455</v>
+        <v>238</v>
       </c>
     </row>
     <row r="33">
       <c r="B33" t="inlineStr">
         <is>
-          <t>Mean</t>
+          <t>Sum</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1340,28 +1368,28 @@
         </is>
       </c>
       <c r="E33" t="n">
-        <v>4188.09375</v>
+        <v>134019</v>
       </c>
       <c r="F33" t="n">
-        <v>698.0521739130435</v>
+        <v>80276</v>
       </c>
       <c r="G33" t="n">
-        <v>935.6473029045643</v>
+        <v>225491</v>
       </c>
       <c r="H33" t="n">
-        <v>1075.943661971831</v>
+        <v>229176</v>
       </c>
       <c r="I33" t="n">
-        <v>887.6615384615385</v>
+        <v>230792</v>
       </c>
       <c r="J33" t="n">
-        <v>1073.010695187166</v>
+        <v>200653</v>
       </c>
       <c r="K33" t="n">
-        <v>1231.508771929825</v>
+        <v>210588</v>
       </c>
       <c r="L33" t="n">
-        <v>7048.392857142857</v>
+        <v>197355</v>
       </c>
     </row>
     <row r="34">
@@ -1371,34 +1399,34 @@
         </is>
       </c>
       <c r="E34" t="n">
-        <v>603.5481171548117</v>
+        <v>144248</v>
       </c>
       <c r="F34" t="n">
         <v>233</v>
       </c>
       <c r="G34" t="n">
-        <v>3255.114754098361</v>
+        <v>198562</v>
       </c>
       <c r="H34" t="n">
-        <v>1956.815789473684</v>
+        <v>223077</v>
       </c>
       <c r="I34" t="n">
-        <v>9988.363636363636</v>
+        <v>219744</v>
       </c>
       <c r="J34" t="n">
-        <v>4276.555555555556</v>
+        <v>192445</v>
       </c>
       <c r="K34" t="n">
-        <v>2183.214285714286</v>
+        <v>213955</v>
       </c>
       <c r="L34" t="n">
-        <v>893.2184873949579</v>
+        <v>212586</v>
       </c>
     </row>
     <row r="35">
       <c r="B35" t="inlineStr">
         <is>
-          <t>Q25</t>
+          <t>Min</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1406,30 +1434,16 @@
           <t>Left</t>
         </is>
       </c>
-      <c r="E35" t="n">
-        <v>1.75</v>
-      </c>
-      <c r="F35" t="n">
-        <v>1</v>
-      </c>
+      <c r="E35" t="inlineStr"/>
+      <c r="F35" t="inlineStr"/>
       <c r="G35" t="n">
-        <v>1</v>
-      </c>
-      <c r="H35" t="n">
-        <v>1</v>
-      </c>
-      <c r="I35" t="n">
-        <v>1</v>
-      </c>
-      <c r="J35" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="K35" t="n">
-        <v>2</v>
-      </c>
-      <c r="L35" t="n">
-        <v>1</v>
-      </c>
+        <v>-57</v>
+      </c>
+      <c r="H35" t="inlineStr"/>
+      <c r="I35" t="inlineStr"/>
+      <c r="J35" t="inlineStr"/>
+      <c r="K35" t="inlineStr"/>
+      <c r="L35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="C36" t="inlineStr">
@@ -1437,35 +1451,21 @@
           <t>Right</t>
         </is>
       </c>
-      <c r="E36" t="n">
-        <v>3</v>
-      </c>
+      <c r="E36" t="inlineStr"/>
       <c r="F36" t="n">
         <v>233</v>
       </c>
-      <c r="G36" t="n">
-        <v>1</v>
-      </c>
-      <c r="H36" t="n">
-        <v>1.25</v>
-      </c>
-      <c r="I36" t="n">
-        <v>4</v>
-      </c>
-      <c r="J36" t="n">
-        <v>13</v>
-      </c>
-      <c r="K36" t="n">
-        <v>1</v>
-      </c>
-      <c r="L36" t="n">
-        <v>1</v>
-      </c>
+      <c r="G36" t="inlineStr"/>
+      <c r="H36" t="inlineStr"/>
+      <c r="I36" t="inlineStr"/>
+      <c r="J36" t="inlineStr"/>
+      <c r="K36" t="inlineStr"/>
+      <c r="L36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="B37" t="inlineStr">
         <is>
-          <t>Q50</t>
+          <t>Max</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1474,28 +1474,28 @@
         </is>
       </c>
       <c r="E37" t="n">
-        <v>6</v>
+        <v>35637</v>
       </c>
       <c r="F37" t="n">
-        <v>2</v>
+        <v>20160</v>
       </c>
       <c r="G37" t="n">
-        <v>3</v>
+        <v>16106</v>
       </c>
       <c r="H37" t="n">
-        <v>5</v>
+        <v>30070</v>
       </c>
       <c r="I37" t="n">
-        <v>2</v>
+        <v>31410</v>
       </c>
       <c r="J37" t="n">
-        <v>57</v>
+        <v>31910</v>
       </c>
       <c r="K37" t="n">
-        <v>4</v>
+        <v>41718</v>
       </c>
       <c r="L37" t="n">
-        <v>6</v>
+        <v>109783</v>
       </c>
     </row>
     <row r="38">
@@ -1505,34 +1505,34 @@
         </is>
       </c>
       <c r="E38" t="n">
-        <v>46</v>
+        <v>21955</v>
       </c>
       <c r="F38" t="n">
         <v>233</v>
       </c>
       <c r="G38" t="n">
-        <v>36</v>
+        <v>42468</v>
       </c>
       <c r="H38" t="n">
-        <v>6</v>
+        <v>38333</v>
       </c>
       <c r="I38" t="n">
-        <v>386</v>
+        <v>72522</v>
       </c>
       <c r="J38" t="n">
-        <v>265</v>
+        <v>38870</v>
       </c>
       <c r="K38" t="n">
-        <v>4</v>
+        <v>51579</v>
       </c>
       <c r="L38" t="n">
-        <v>2</v>
+        <v>46455</v>
       </c>
     </row>
     <row r="39">
       <c r="B39" t="inlineStr">
         <is>
-          <t>Q75</t>
+          <t>Mean</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1541,28 +1541,28 @@
         </is>
       </c>
       <c r="E39" t="n">
-        <v>3672.25</v>
+        <v>4188.09375</v>
       </c>
       <c r="F39" t="n">
-        <v>7</v>
+        <v>698.0521739130435</v>
       </c>
       <c r="G39" t="n">
-        <v>213</v>
+        <v>935.6473029045643</v>
       </c>
       <c r="H39" t="n">
-        <v>438</v>
+        <v>1075.943661971831</v>
       </c>
       <c r="I39" t="n">
-        <v>8</v>
+        <v>887.6615384615385</v>
       </c>
       <c r="J39" t="n">
-        <v>676.5</v>
+        <v>1073.010695187166</v>
       </c>
       <c r="K39" t="n">
-        <v>66.5</v>
+        <v>1231.508771929825</v>
       </c>
       <c r="L39" t="n">
-        <v>1657.5</v>
+        <v>7048.392857142857</v>
       </c>
     </row>
     <row r="40">
@@ -1572,34 +1572,34 @@
         </is>
       </c>
       <c r="E40" t="n">
-        <v>174.5</v>
+        <v>603.5481171548117</v>
       </c>
       <c r="F40" t="n">
         <v>233</v>
       </c>
       <c r="G40" t="n">
-        <v>1300</v>
+        <v>3255.114754098361</v>
       </c>
       <c r="H40" t="n">
-        <v>636.5</v>
+        <v>1956.815789473684</v>
       </c>
       <c r="I40" t="n">
-        <v>11211.75</v>
+        <v>9988.363636363636</v>
       </c>
       <c r="J40" t="n">
-        <v>2840</v>
+        <v>4276.555555555556</v>
       </c>
       <c r="K40" t="n">
-        <v>205.25</v>
+        <v>2183.214285714286</v>
       </c>
       <c r="L40" t="n">
-        <v>28</v>
+        <v>893.2184873949579</v>
       </c>
     </row>
     <row r="41">
       <c r="B41" t="inlineStr">
         <is>
-          <t>IQR</t>
+          <t>Q25</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1608,28 +1608,28 @@
         </is>
       </c>
       <c r="E41" t="n">
-        <v>3670.5</v>
+        <v>1.75</v>
       </c>
       <c r="F41" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G41" t="n">
-        <v>212</v>
+        <v>1</v>
       </c>
       <c r="H41" t="n">
-        <v>437</v>
+        <v>1</v>
       </c>
       <c r="I41" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="J41" t="n">
-        <v>672</v>
+        <v>4.5</v>
       </c>
       <c r="K41" t="n">
-        <v>64.5</v>
+        <v>2</v>
       </c>
       <c r="L41" t="n">
-        <v>1656.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42">
@@ -1639,26 +1639,1013 @@
         </is>
       </c>
       <c r="E42" t="n">
+        <v>3</v>
+      </c>
+      <c r="F42" t="n">
+        <v>233</v>
+      </c>
+      <c r="G42" t="n">
+        <v>1</v>
+      </c>
+      <c r="H42" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="I42" t="n">
+        <v>4</v>
+      </c>
+      <c r="J42" t="n">
+        <v>13</v>
+      </c>
+      <c r="K42" t="n">
+        <v>1</v>
+      </c>
+      <c r="L42" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Q50</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Left</t>
+        </is>
+      </c>
+      <c r="E43" t="n">
+        <v>6</v>
+      </c>
+      <c r="F43" t="n">
+        <v>2</v>
+      </c>
+      <c r="G43" t="n">
+        <v>3</v>
+      </c>
+      <c r="H43" t="n">
+        <v>5</v>
+      </c>
+      <c r="I43" t="n">
+        <v>2</v>
+      </c>
+      <c r="J43" t="n">
+        <v>57</v>
+      </c>
+      <c r="K43" t="n">
+        <v>4</v>
+      </c>
+      <c r="L43" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Right</t>
+        </is>
+      </c>
+      <c r="E44" t="n">
+        <v>46</v>
+      </c>
+      <c r="F44" t="n">
+        <v>233</v>
+      </c>
+      <c r="G44" t="n">
+        <v>36</v>
+      </c>
+      <c r="H44" t="n">
+        <v>6</v>
+      </c>
+      <c r="I44" t="n">
+        <v>386</v>
+      </c>
+      <c r="J44" t="n">
+        <v>265</v>
+      </c>
+      <c r="K44" t="n">
+        <v>4</v>
+      </c>
+      <c r="L44" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Q75</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Left</t>
+        </is>
+      </c>
+      <c r="E45" t="n">
+        <v>3672.25</v>
+      </c>
+      <c r="F45" t="n">
+        <v>7</v>
+      </c>
+      <c r="G45" t="n">
+        <v>213</v>
+      </c>
+      <c r="H45" t="n">
+        <v>438</v>
+      </c>
+      <c r="I45" t="n">
+        <v>8</v>
+      </c>
+      <c r="J45" t="n">
+        <v>676.5</v>
+      </c>
+      <c r="K45" t="n">
+        <v>66.5</v>
+      </c>
+      <c r="L45" t="n">
+        <v>1657.5</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Right</t>
+        </is>
+      </c>
+      <c r="E46" t="n">
+        <v>174.5</v>
+      </c>
+      <c r="F46" t="n">
+        <v>233</v>
+      </c>
+      <c r="G46" t="n">
+        <v>1300</v>
+      </c>
+      <c r="H46" t="n">
+        <v>636.5</v>
+      </c>
+      <c r="I46" t="n">
+        <v>11211.75</v>
+      </c>
+      <c r="J46" t="n">
+        <v>2840</v>
+      </c>
+      <c r="K46" t="n">
+        <v>205.25</v>
+      </c>
+      <c r="L46" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>IQR</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Left</t>
+        </is>
+      </c>
+      <c r="E47" t="n">
+        <v>3670.5</v>
+      </c>
+      <c r="F47" t="n">
+        <v>6</v>
+      </c>
+      <c r="G47" t="n">
+        <v>212</v>
+      </c>
+      <c r="H47" t="n">
+        <v>437</v>
+      </c>
+      <c r="I47" t="n">
+        <v>7</v>
+      </c>
+      <c r="J47" t="n">
+        <v>672</v>
+      </c>
+      <c r="K47" t="n">
+        <v>64.5</v>
+      </c>
+      <c r="L47" t="n">
+        <v>1656.5</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Right</t>
+        </is>
+      </c>
+      <c r="E48" t="n">
         <v>171.5</v>
       </c>
-      <c r="F42" t="inlineStr"/>
-      <c r="G42" t="n">
+      <c r="F48" t="inlineStr"/>
+      <c r="G48" t="n">
         <v>1299</v>
       </c>
-      <c r="H42" t="n">
+      <c r="H48" t="n">
         <v>635.25</v>
       </c>
-      <c r="I42" t="n">
+      <c r="I48" t="n">
         <v>11207.75</v>
       </c>
-      <c r="J42" t="n">
+      <c r="J48" t="n">
         <v>2827</v>
       </c>
-      <c r="K42" t="n">
+      <c r="K48" t="n">
         <v>204.25</v>
       </c>
-      <c r="L42" t="n">
+      <c r="L48" t="n">
         <v>27</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>P90</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Left</t>
+        </is>
+      </c>
+      <c r="E49" t="n">
+        <v>12101.40000000001</v>
+      </c>
+      <c r="F49" t="n">
+        <v>1080.000000000001</v>
+      </c>
+      <c r="G49" t="n">
+        <v>2362</v>
+      </c>
+      <c r="H49" t="n">
+        <v>3865.600000000004</v>
+      </c>
+      <c r="I49" t="n">
+        <v>2538.199999999994</v>
+      </c>
+      <c r="J49" t="n">
+        <v>3306.800000000006</v>
+      </c>
+      <c r="K49" t="n">
+        <v>2672</v>
+      </c>
+      <c r="L49" t="n">
+        <v>6433.500000000004</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Right</t>
+        </is>
+      </c>
+      <c r="E50" t="n">
+        <v>1267</v>
+      </c>
+      <c r="F50" t="n">
+        <v>233</v>
+      </c>
+      <c r="G50" t="n">
+        <v>10735</v>
+      </c>
+      <c r="H50" t="n">
+        <v>6212.100000000001</v>
+      </c>
+      <c r="I50" t="n">
+        <v>37983.20000000006</v>
+      </c>
+      <c r="J50" t="n">
+        <v>12794.00000000001</v>
+      </c>
+      <c r="K50" t="n">
+        <v>5702.299999999999</v>
+      </c>
+      <c r="L50" t="n">
+        <v>1418.000000000001</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>P95</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Left</t>
+        </is>
+      </c>
+      <c r="E51" t="n">
+        <v>22865.39999999999</v>
+      </c>
+      <c r="F51" t="n">
+        <v>3957.699999999993</v>
+      </c>
+      <c r="G51" t="n">
+        <v>6554</v>
+      </c>
+      <c r="H51" t="n">
+        <v>5702.599999999992</v>
+      </c>
+      <c r="I51" t="n">
+        <v>5465.25</v>
+      </c>
+      <c r="J51" t="n">
+        <v>5377.699999999999</v>
+      </c>
+      <c r="K51" t="n">
+        <v>4819</v>
+      </c>
+      <c r="L51" t="n">
+        <v>41537.44999999993</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Right</t>
+        </is>
+      </c>
+      <c r="E52" t="n">
+        <v>2502.099999999998</v>
+      </c>
+      <c r="F52" t="n">
+        <v>233</v>
+      </c>
+      <c r="G52" t="n">
+        <v>16654</v>
+      </c>
+      <c r="H52" t="n">
+        <v>11803.64999999998</v>
+      </c>
+      <c r="I52" t="n">
+        <v>46392.35</v>
+      </c>
+      <c r="J52" t="n">
+        <v>31503.59999999998</v>
+      </c>
+      <c r="K52" t="n">
+        <v>10505.3</v>
+      </c>
+      <c r="L52" t="n">
+        <v>4165.849999999987</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>P99</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Left</t>
+        </is>
+      </c>
+      <c r="E53" t="n">
+        <v>33558.76000000001</v>
+      </c>
+      <c r="F53" t="n">
+        <v>12690.72</v>
+      </c>
+      <c r="G53" t="n">
+        <v>14140.99999999999</v>
+      </c>
+      <c r="H53" t="n">
+        <v>12022.59999999999</v>
+      </c>
+      <c r="I53" t="n">
+        <v>12999.66000000004</v>
+      </c>
+      <c r="J53" t="n">
+        <v>10065.43999999983</v>
+      </c>
+      <c r="K53" t="n">
+        <v>25414.60000000025</v>
+      </c>
+      <c r="L53" t="n">
+        <v>95999.77000000002</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Right</t>
+        </is>
+      </c>
+      <c r="E54" t="n">
+        <v>10486.60000000003</v>
+      </c>
+      <c r="F54" t="n">
+        <v>233</v>
+      </c>
+      <c r="G54" t="n">
+        <v>41598.6</v>
+      </c>
+      <c r="H54" t="n">
+        <v>26169.16000000005</v>
+      </c>
+      <c r="I54" t="n">
+        <v>67096.85999999997</v>
+      </c>
+      <c r="J54" t="n">
+        <v>37372.24000000001</v>
+      </c>
+      <c r="K54" t="n">
+        <v>47926.95</v>
+      </c>
+      <c r="L54" t="n">
+        <v>19620.81999999999</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="E58" t="n">
+        <v>1</v>
+      </c>
+      <c r="F58" t="n">
+        <v>3</v>
+      </c>
+      <c r="G58" t="n">
+        <v>5</v>
+      </c>
+      <c r="H58" t="n">
+        <v>6</v>
+      </c>
+      <c r="I58" t="n">
+        <v>7</v>
+      </c>
+      <c r="J58" t="n">
+        <v>8</v>
+      </c>
+      <c r="K58" t="n">
+        <v>9</v>
+      </c>
+      <c r="L58" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Left</t>
+        </is>
+      </c>
+      <c r="E59" t="n">
+        <v>273</v>
+      </c>
+      <c r="F59" t="n">
+        <v>118</v>
+      </c>
+      <c r="G59" t="n">
+        <v>304</v>
+      </c>
+      <c r="H59" t="n">
+        <v>329</v>
+      </c>
+      <c r="I59" t="n">
+        <v>284</v>
+      </c>
+      <c r="J59" t="n">
+        <v>234</v>
+      </c>
+      <c r="K59" t="n">
+        <v>271</v>
+      </c>
+      <c r="L59" t="n">
+        <v>268</v>
+      </c>
+      <c r="M59" t="n">
+        <v>2081</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Right</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Sum</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Left</t>
+        </is>
+      </c>
+      <c r="E61" t="n">
+        <v>1765273</v>
+      </c>
+      <c r="F61" t="n">
+        <v>80858</v>
+      </c>
+      <c r="G61" t="n">
+        <v>532799</v>
+      </c>
+      <c r="H61" t="n">
+        <v>3315679</v>
+      </c>
+      <c r="I61" t="n">
+        <v>411108</v>
+      </c>
+      <c r="J61" t="n">
+        <v>4872290</v>
+      </c>
+      <c r="K61" t="n">
+        <v>3469821</v>
+      </c>
+      <c r="L61" t="n">
+        <v>210958</v>
+      </c>
+      <c r="M61" t="n">
+        <v>14658786</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Right</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Min</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Left</t>
+        </is>
+      </c>
+      <c r="E63" t="n">
+        <v>462</v>
+      </c>
+      <c r="F63" t="n">
+        <v>464</v>
+      </c>
+      <c r="G63" t="n">
+        <v>459</v>
+      </c>
+      <c r="H63" t="n">
+        <v>463</v>
+      </c>
+      <c r="I63" t="n">
+        <v>461</v>
+      </c>
+      <c r="J63" t="n">
+        <v>461</v>
+      </c>
+      <c r="K63" t="n">
+        <v>463</v>
+      </c>
+      <c r="L63" t="n">
+        <v>462</v>
+      </c>
+      <c r="M63" t="n">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Right</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Max</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Left</t>
+        </is>
+      </c>
+      <c r="E65" t="n">
+        <v>907406</v>
+      </c>
+      <c r="F65" t="n">
+        <v>6734</v>
+      </c>
+      <c r="G65" t="n">
+        <v>206746</v>
+      </c>
+      <c r="H65" t="n">
+        <v>1126123</v>
+      </c>
+      <c r="I65" t="n">
+        <v>16527</v>
+      </c>
+      <c r="J65" t="n">
+        <v>3808470</v>
+      </c>
+      <c r="K65" t="n">
+        <v>2844365</v>
+      </c>
+      <c r="L65" t="n">
+        <v>36436</v>
+      </c>
+      <c r="M65" t="n">
+        <v>3808470</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Right</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>Mean</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Left</t>
+        </is>
+      </c>
+      <c r="E67" t="n">
+        <v>6466.201465201465</v>
+      </c>
+      <c r="F67" t="n">
+        <v>685.2372881355932</v>
+      </c>
+      <c r="G67" t="n">
+        <v>1752.628289473684</v>
+      </c>
+      <c r="H67" t="n">
+        <v>10078.05167173252</v>
+      </c>
+      <c r="I67" t="n">
+        <v>1447.56338028169</v>
+      </c>
+      <c r="J67" t="n">
+        <v>20821.75213675214</v>
+      </c>
+      <c r="K67" t="n">
+        <v>12803.76752767528</v>
+      </c>
+      <c r="L67" t="n">
+        <v>787.1567164179105</v>
+      </c>
+      <c r="M67" t="n">
+        <v>7044.106679481019</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Right</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>Q25</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Left</t>
+        </is>
+      </c>
+      <c r="E69" t="n">
+        <v>470</v>
+      </c>
+      <c r="F69" t="n">
+        <v>476</v>
+      </c>
+      <c r="G69" t="n">
+        <v>470</v>
+      </c>
+      <c r="H69" t="n">
+        <v>471</v>
+      </c>
+      <c r="I69" t="n">
+        <v>476</v>
+      </c>
+      <c r="J69" t="n">
+        <v>470</v>
+      </c>
+      <c r="K69" t="n">
+        <v>470</v>
+      </c>
+      <c r="L69" t="n">
+        <v>470</v>
+      </c>
+      <c r="M69" t="n">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>Right</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>Q50</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>Left</t>
+        </is>
+      </c>
+      <c r="E71" t="n">
+        <v>470</v>
+      </c>
+      <c r="F71" t="n">
+        <v>477</v>
+      </c>
+      <c r="G71" t="n">
+        <v>476</v>
+      </c>
+      <c r="H71" t="n">
+        <v>488</v>
+      </c>
+      <c r="I71" t="n">
+        <v>479</v>
+      </c>
+      <c r="J71" t="n">
+        <v>471</v>
+      </c>
+      <c r="K71" t="n">
+        <v>478</v>
+      </c>
+      <c r="L71" t="n">
+        <v>471</v>
+      </c>
+      <c r="M71" t="n">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>Right</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>Q75</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>Left</t>
+        </is>
+      </c>
+      <c r="E73" t="n">
+        <v>479</v>
+      </c>
+      <c r="F73" t="n">
+        <v>477.75</v>
+      </c>
+      <c r="G73" t="n">
+        <v>585</v>
+      </c>
+      <c r="H73" t="n">
+        <v>2397</v>
+      </c>
+      <c r="I73" t="n">
+        <v>1133.5</v>
+      </c>
+      <c r="J73" t="n">
+        <v>913.5</v>
+      </c>
+      <c r="K73" t="n">
+        <v>721</v>
+      </c>
+      <c r="L73" t="n">
+        <v>479.25</v>
+      </c>
+      <c r="M73" t="n">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Right</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>IQR</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>Left</t>
+        </is>
+      </c>
+      <c r="E75" t="n">
+        <v>9</v>
+      </c>
+      <c r="F75" t="n">
+        <v>1.75</v>
+      </c>
+      <c r="G75" t="n">
+        <v>115</v>
+      </c>
+      <c r="H75" t="n">
+        <v>1926</v>
+      </c>
+      <c r="I75" t="n">
+        <v>657.5</v>
+      </c>
+      <c r="J75" t="n">
+        <v>443.5</v>
+      </c>
+      <c r="K75" t="n">
+        <v>251</v>
+      </c>
+      <c r="L75" t="n">
+        <v>9.25</v>
+      </c>
+      <c r="M75" t="n">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>Right</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>P90</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>Left</t>
+        </is>
+      </c>
+      <c r="E77" t="n">
+        <v>543.8000000000002</v>
+      </c>
+      <c r="F77" t="n">
+        <v>593</v>
+      </c>
+      <c r="G77" t="n">
+        <v>1019.8</v>
+      </c>
+      <c r="H77" t="n">
+        <v>8630.799999999997</v>
+      </c>
+      <c r="I77" t="n">
+        <v>4000.500000000001</v>
+      </c>
+      <c r="J77" t="n">
+        <v>4604.400000000001</v>
+      </c>
+      <c r="K77" t="n">
+        <v>1891</v>
+      </c>
+      <c r="L77" t="n">
+        <v>798.9000000000001</v>
+      </c>
+      <c r="M77" t="n">
+        <v>2355</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>Right</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>P95</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>Left</t>
+        </is>
+      </c>
+      <c r="E79" t="n">
+        <v>799.5999999999999</v>
+      </c>
+      <c r="F79" t="n">
+        <v>1353.399999999996</v>
+      </c>
+      <c r="G79" t="n">
+        <v>1866.85</v>
+      </c>
+      <c r="H79" t="n">
+        <v>13969.6</v>
+      </c>
+      <c r="I79" t="n">
+        <v>5763.899999999996</v>
+      </c>
+      <c r="J79" t="n">
+        <v>8586.949999999997</v>
+      </c>
+      <c r="K79" t="n">
+        <v>3800</v>
+      </c>
+      <c r="L79" t="n">
+        <v>1404.449999999999</v>
+      </c>
+      <c r="M79" t="n">
+        <v>5888</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>Right</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>P99</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>Left</t>
+        </is>
+      </c>
+      <c r="E81" t="n">
+        <v>7908.039999999732</v>
+      </c>
+      <c r="F81" t="n">
+        <v>6129.199999999997</v>
+      </c>
+      <c r="G81" t="n">
+        <v>12073.15999999991</v>
+      </c>
+      <c r="H81" t="n">
+        <v>268149.2799999971</v>
+      </c>
+      <c r="I81" t="n">
+        <v>10275.53000000002</v>
+      </c>
+      <c r="J81" t="n">
+        <v>208288.3099999973</v>
+      </c>
+      <c r="K81" t="n">
+        <v>26141.20000000036</v>
+      </c>
+      <c r="L81" t="n">
+        <v>5134.959999999949</v>
+      </c>
+      <c r="M81" t="n">
+        <v>21227.59999999959</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>Right</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>